<commit_message>
working on inserting employee
</commit_message>
<xml_diff>
--- a/übersicht Auslastung Jan_Dez2019.xlsx
+++ b/übersicht Auslastung Jan_Dez2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanessakrueger/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mobile/go/src/github.com/AnotherCoolDude/workload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768559A0-E2A3-194C-A74D-7C9A90F03E6F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF37C95-E9DC-4046-881F-E68C6860ABD2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="800" windowWidth="45620" windowHeight="27220" tabRatio="713" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16760" tabRatio="713" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kundenjobs" sheetId="9" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -2477,7 +2478,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8148D356-48E5-064D-BBD8-0DC9D38227B7}">
   <dimension ref="A1:BB67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="120" workbookViewId="0">
@@ -3239,7 +3240,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A9" s="28" t="s">
         <v>58</v>
       </c>
@@ -5667,7 +5668,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="31" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
         <v>93</v>
       </c>
@@ -5774,7 +5775,7 @@
         <v>689.75</v>
       </c>
     </row>
-    <row r="32" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
         <v>83</v>
       </c>
@@ -6948,7 +6949,7 @@
         <v>257.5</v>
       </c>
     </row>
-    <row r="42" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A42" s="5" t="s">
         <v>23</v>
       </c>
@@ -7240,7 +7241,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A45" s="5" t="s">
         <v>25</v>
       </c>
@@ -8000,7 +8001,7 @@
         <v>36.049999999999997</v>
       </c>
     </row>
-    <row r="51" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A51" s="5" t="s">
         <v>82</v>
       </c>
@@ -8941,7 +8942,7 @@
       <c r="BA58" s="16"/>
       <c r="BB58" s="8"/>
     </row>
-    <row r="59" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A59" s="5" t="s">
         <v>92</v>
       </c>
@@ -9037,7 +9038,7 @@
         <v>466.5</v>
       </c>
     </row>
-    <row r="60" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A60" s="5" t="s">
         <v>99</v>
       </c>
@@ -9111,7 +9112,7 @@
         <v>325.25</v>
       </c>
     </row>
-    <row r="61" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A61" s="5" t="s">
         <v>100</v>
       </c>
@@ -9181,7 +9182,7 @@
         <v>159.5</v>
       </c>
     </row>
-    <row r="62" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A62" s="129" t="s">
         <v>85</v>
       </c>
@@ -9255,7 +9256,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="63" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
         <v>86</v>
       </c>
@@ -9349,7 +9350,7 @@
         <v>339.25</v>
       </c>
     </row>
-    <row r="64" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
         <v>87</v>
       </c>
@@ -9660,7 +9661,7 @@
         <v>2223.5</v>
       </c>
     </row>
-    <row r="66" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A66" s="5"/>
       <c r="B66" s="24"/>
       <c r="C66" s="24"/>
@@ -9909,7 +9910,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C8CF26-71A3-D14C-9A10-BFE7F88F3A01}">
   <dimension ref="A1:CQ73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9966,7 +9967,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -9981,7 +9982,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -10008,12 +10009,12 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A11" s="5"/>
       <c r="B11" s="83"/>
       <c r="C11" s="83"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
@@ -10028,7 +10029,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A13" s="122" t="s">
         <v>97</v>
       </c>
@@ -10043,7 +10044,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
@@ -10058,7 +10059,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
@@ -10073,7 +10074,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
@@ -10088,7 +10089,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
         <v>76</v>
       </c>
@@ -10103,7 +10104,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A18" s="129" t="s">
         <v>59</v>
       </c>
@@ -10118,7 +10119,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A19" s="5" t="s">
         <v>77</v>
       </c>
@@ -10133,7 +10134,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A20" s="5" t="s">
         <v>84</v>
       </c>
@@ -10148,7 +10149,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
         <v>11</v>
       </c>
@@ -10163,7 +10164,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
         <v>79</v>
       </c>
@@ -10195,7 +10196,7 @@
       <c r="C24" s="83"/>
       <c r="D24" s="83"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A25" s="32" t="s">
         <v>91</v>
       </c>
@@ -10210,7 +10211,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
         <v>13</v>
       </c>
@@ -10226,7 +10227,7 @@
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
         <v>15</v>
       </c>
@@ -10241,7 +10242,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
         <v>95</v>
       </c>
@@ -10256,7 +10257,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
         <v>90</v>
       </c>
@@ -10271,7 +10272,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A30" s="36" t="s">
         <v>80</v>
       </c>
@@ -10286,7 +10287,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
         <v>16</v>
       </c>
@@ -10301,7 +10302,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="25" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
         <v>83</v>
       </c>
@@ -10316,7 +10317,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="25" x14ac:dyDescent="0.4">
       <c r="A33" s="5" t="s">
         <v>17</v>
       </c>
@@ -10331,7 +10332,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="25" x14ac:dyDescent="0.4">
       <c r="A34" s="9" t="s">
         <v>18</v>
       </c>
@@ -10346,7 +10347,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="25" x14ac:dyDescent="0.4">
       <c r="A35" s="9" t="s">
         <v>81</v>
       </c>
@@ -10361,7 +10362,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="25" x14ac:dyDescent="0.4">
       <c r="A36" s="33" t="s">
         <v>19</v>
       </c>
@@ -10372,13 +10373,13 @@
         <v>8970</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="25" x14ac:dyDescent="0.4">
       <c r="A37" s="5"/>
       <c r="B37" s="83"/>
       <c r="C37" s="85"/>
       <c r="D37" s="83"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="25" x14ac:dyDescent="0.4">
       <c r="A38" s="129" t="s">
         <v>20</v>
       </c>
@@ -10404,13 +10405,13 @@
         <v>640</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="25" x14ac:dyDescent="0.4">
       <c r="A40" s="5"/>
       <c r="B40" s="84"/>
       <c r="C40" s="84"/>
       <c r="D40" s="84"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="25" x14ac:dyDescent="0.4">
       <c r="A41" s="5" t="s">
         <v>22</v>
       </c>
@@ -10425,7 +10426,7 @@
         <v>747.5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="25" x14ac:dyDescent="0.4">
       <c r="A42" s="5" t="s">
         <v>23</v>
       </c>
@@ -10440,7 +10441,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="25" x14ac:dyDescent="0.4">
       <c r="A43" s="5" t="s">
         <v>24</v>
       </c>
@@ -10455,7 +10456,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="25" x14ac:dyDescent="0.4">
       <c r="A44" s="127" t="s">
         <v>98</v>
       </c>
@@ -10470,7 +10471,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="25" x14ac:dyDescent="0.4">
       <c r="A45" s="5" t="s">
         <v>25</v>
       </c>
@@ -10496,7 +10497,7 @@
         <v>3062.5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="26" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A47" s="5"/>
       <c r="B47" s="83"/>
       <c r="C47" s="85"/>
@@ -10610,7 +10611,7 @@
       <c r="CP49" s="17"/>
       <c r="CQ49" s="17"/>
     </row>
-    <row r="50" spans="1:95" s="13" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:95" s="13" customFormat="1" ht="26" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A50" s="5" t="s">
         <v>31</v>
       </c>
@@ -10716,7 +10717,7 @@
       <c r="CP50" s="17"/>
       <c r="CQ50" s="17"/>
     </row>
-    <row r="51" spans="1:95" s="17" customFormat="1" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:95" s="17" customFormat="1" ht="26" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A51" s="5" t="s">
         <v>82</v>
       </c>
@@ -10731,7 +10732,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="52" spans="1:95" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:95" s="17" customFormat="1" ht="25" x14ac:dyDescent="0.4">
       <c r="A52" s="5" t="s">
         <v>32</v>
       </c>
@@ -10757,13 +10758,13 @@
         <v>2668</v>
       </c>
     </row>
-    <row r="54" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:95" ht="25" x14ac:dyDescent="0.4">
       <c r="A54" s="5"/>
       <c r="B54" s="83"/>
       <c r="C54" s="83"/>
       <c r="D54" s="83"/>
     </row>
-    <row r="55" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:95" ht="25" x14ac:dyDescent="0.4">
       <c r="A55" s="5" t="s">
         <v>89</v>
       </c>
@@ -10778,7 +10779,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="56" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:95" ht="25" x14ac:dyDescent="0.4">
       <c r="A56" s="129" t="s">
         <v>34</v>
       </c>
@@ -10810,7 +10811,7 @@
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
     </row>
-    <row r="59" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:95" ht="25" x14ac:dyDescent="0.4">
       <c r="A59" s="5" t="s">
         <v>92</v>
       </c>
@@ -10825,7 +10826,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="60" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:95" ht="25" x14ac:dyDescent="0.4">
       <c r="A60" s="122" t="s">
         <v>99</v>
       </c>
@@ -10840,7 +10841,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="61" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:95" ht="25" x14ac:dyDescent="0.4">
       <c r="A61" s="122" t="s">
         <v>100</v>
       </c>
@@ -10855,7 +10856,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="62" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:95" ht="25" x14ac:dyDescent="0.4">
       <c r="A62" s="129" t="s">
         <v>85</v>
       </c>
@@ -10870,7 +10871,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="63" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:95" ht="25" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
         <v>86</v>
       </c>
@@ -10885,7 +10886,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="64" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:95" ht="25" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
         <v>87</v>
       </c>
@@ -10911,7 +10912,7 @@
         <v>3660</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="26" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A66" s="5"/>
       <c r="B66" s="83"/>
       <c r="C66" s="85"/>
@@ -10971,7 +10972,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0714548-41A8-6F42-A747-789E6D284EE1}">
   <dimension ref="A1:BB67"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="120" workbookViewId="0">
@@ -11731,7 +11732,7 @@
         <v>74.75</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A9" s="28" t="s">
         <v>58</v>
       </c>
@@ -14147,7 +14148,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="31" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
         <v>93</v>
       </c>
@@ -14254,7 +14255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
         <v>83</v>
       </c>
@@ -15428,7 +15429,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A42" s="5" t="s">
         <v>23</v>
       </c>
@@ -15718,7 +15719,7 @@
       <c r="BA44" s="21"/>
       <c r="BB44" s="6"/>
     </row>
-    <row r="45" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A45" s="5" t="s">
         <v>25</v>
       </c>
@@ -16478,7 +16479,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="51" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A51" s="5" t="s">
         <v>82</v>
       </c>
@@ -16951,7 +16952,7 @@
       <c r="AM54" s="19"/>
       <c r="BB54" s="6"/>
     </row>
-    <row r="55" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A55" s="5" t="s">
         <v>89</v>
       </c>
@@ -17047,7 +17048,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="56" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A56" s="129" t="s">
         <v>34</v>
       </c>
@@ -17419,7 +17420,7 @@
       <c r="BA58" s="16"/>
       <c r="BB58" s="8"/>
     </row>
-    <row r="59" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A59" s="5" t="s">
         <v>92</v>
       </c>
@@ -17515,7 +17516,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A60" s="5" t="s">
         <v>99</v>
       </c>
@@ -17586,7 +17587,7 @@
       <c r="BA60" s="106"/>
       <c r="BB60" s="105"/>
     </row>
-    <row r="61" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A61" s="5" t="s">
         <v>100</v>
       </c>
@@ -17653,7 +17654,7 @@
       <c r="BA61" s="106"/>
       <c r="BB61" s="105"/>
     </row>
-    <row r="62" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A62" s="129" t="s">
         <v>85</v>
       </c>
@@ -17727,7 +17728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
         <v>86</v>
       </c>
@@ -17821,7 +17822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
         <v>87</v>
       </c>
@@ -18132,7 +18133,7 @@
         <v>56.5</v>
       </c>
     </row>
-    <row r="66" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A66" s="5"/>
       <c r="B66" s="24"/>
       <c r="C66" s="24"/>
@@ -18381,7 +18382,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86AEF284-50C4-9143-8F1F-810B8F0F5145}">
   <dimension ref="A1:BB67"/>
   <sheetViews>
     <sheetView zoomScale="79" zoomScaleNormal="79" zoomScalePageLayoutView="120" workbookViewId="0">
@@ -19145,7 +19146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A9" s="28" t="s">
         <v>58</v>
       </c>
@@ -21552,7 +21553,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="31" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
         <v>93</v>
       </c>
@@ -21659,7 +21660,7 @@
         <v>59.5</v>
       </c>
     </row>
-    <row r="32" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
         <v>83</v>
       </c>
@@ -22833,7 +22834,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="42" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A42" s="5" t="s">
         <v>23</v>
       </c>
@@ -23123,7 +23124,7 @@
       <c r="BA44" s="21"/>
       <c r="BB44" s="6"/>
     </row>
-    <row r="45" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A45" s="5" t="s">
         <v>25</v>
       </c>
@@ -23883,7 +23884,7 @@
         <v>5.45</v>
       </c>
     </row>
-    <row r="51" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A51" s="5" t="s">
         <v>82</v>
       </c>
@@ -24991,7 +24992,7 @@
       <c r="BA60" s="106"/>
       <c r="BB60" s="105"/>
     </row>
-    <row r="61" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A61" s="5" t="s">
         <v>100</v>
       </c>
@@ -25058,7 +25059,7 @@
       <c r="BA61" s="106"/>
       <c r="BB61" s="105"/>
     </row>
-    <row r="62" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A62" s="129" t="s">
         <v>85</v>
       </c>
@@ -25132,7 +25133,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="63" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
         <v>86</v>
       </c>
@@ -25226,7 +25227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
         <v>87</v>
       </c>
@@ -25531,7 +25532,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="66" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A66" s="5"/>
       <c r="B66" s="24"/>
       <c r="C66" s="24"/>
@@ -25780,7 +25781,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42BA62F4-F68A-454A-A23C-02B0040E6B1B}">
   <dimension ref="A1:BB67"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="120" workbookViewId="0">
@@ -26540,7 +26541,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A9" s="28" t="s">
         <v>58</v>
       </c>
@@ -28956,7 +28957,7 @@
         <v>47.5</v>
       </c>
     </row>
-    <row r="31" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
         <v>93</v>
       </c>
@@ -29063,7 +29064,7 @@
         <v>75.25</v>
       </c>
     </row>
-    <row r="32" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
         <v>83</v>
       </c>
@@ -30237,7 +30238,7 @@
         <v>272.5</v>
       </c>
     </row>
-    <row r="42" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A42" s="5" t="s">
         <v>23</v>
       </c>
@@ -30527,7 +30528,7 @@
       <c r="BA44" s="21"/>
       <c r="BB44" s="6"/>
     </row>
-    <row r="45" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A45" s="5" t="s">
         <v>25</v>
       </c>
@@ -31287,7 +31288,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="51" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A51" s="5" t="s">
         <v>82</v>
       </c>
@@ -31760,7 +31761,7 @@
       <c r="AM54" s="19"/>
       <c r="BB54" s="6"/>
     </row>
-    <row r="55" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A55" s="5" t="s">
         <v>89</v>
       </c>
@@ -31856,7 +31857,7 @@
         <v>336.5</v>
       </c>
     </row>
-    <row r="56" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A56" s="129" t="s">
         <v>34</v>
       </c>
@@ -32228,7 +32229,7 @@
       <c r="BA58" s="16"/>
       <c r="BB58" s="8"/>
     </row>
-    <row r="59" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A59" s="5" t="s">
         <v>92</v>
       </c>
@@ -32324,7 +32325,7 @@
         <v>210.5</v>
       </c>
     </row>
-    <row r="60" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A60" s="5" t="s">
         <v>99</v>
       </c>
@@ -32395,7 +32396,7 @@
       <c r="BA60" s="106"/>
       <c r="BB60" s="105"/>
     </row>
-    <row r="61" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A61" s="5" t="s">
         <v>100</v>
       </c>
@@ -32462,7 +32463,7 @@
       <c r="BA61" s="106"/>
       <c r="BB61" s="105"/>
     </row>
-    <row r="62" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A62" s="129" t="s">
         <v>85</v>
       </c>
@@ -32538,7 +32539,7 @@
         <v>120.5</v>
       </c>
     </row>
-    <row r="63" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
         <v>86</v>
       </c>
@@ -32632,7 +32633,7 @@
         <v>161.25</v>
       </c>
     </row>
-    <row r="64" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
         <v>87</v>
       </c>
@@ -32943,7 +32944,7 @@
         <v>638.25</v>
       </c>
     </row>
-    <row r="66" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A66" s="5"/>
       <c r="B66" s="24"/>
       <c r="C66" s="24"/>
@@ -33192,7 +33193,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE447B5-D05F-DB4A-A972-2484570794B0}">
   <dimension ref="A1:BB67"/>
   <sheetViews>
     <sheetView zoomScale="93" zoomScaleNormal="93" zoomScalePageLayoutView="120" workbookViewId="0">
@@ -33951,7 +33952,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A9" s="28" t="s">
         <v>58</v>
       </c>
@@ -36369,7 +36370,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
         <v>93</v>
       </c>
@@ -36476,7 +36477,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
         <v>83</v>
       </c>
@@ -37650,7 +37651,7 @@
         <v>71.5</v>
       </c>
     </row>
-    <row r="42" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A42" s="5" t="s">
         <v>23</v>
       </c>
@@ -37940,7 +37941,7 @@
       <c r="BA44" s="21"/>
       <c r="BB44" s="6"/>
     </row>
-    <row r="45" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A45" s="5" t="s">
         <v>25</v>
       </c>
@@ -38700,7 +38701,7 @@
         <v>50.5</v>
       </c>
     </row>
-    <row r="51" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A51" s="5" t="s">
         <v>82</v>
       </c>
@@ -39641,7 +39642,7 @@
       <c r="BA58" s="16"/>
       <c r="BB58" s="8"/>
     </row>
-    <row r="59" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A59" s="5" t="s">
         <v>92</v>
       </c>
@@ -39737,7 +39738,7 @@
         <v>53.5</v>
       </c>
     </row>
-    <row r="60" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A60" s="5" t="s">
         <v>99</v>
       </c>
@@ -39808,7 +39809,7 @@
       <c r="BA60" s="106"/>
       <c r="BB60" s="105"/>
     </row>
-    <row r="61" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A61" s="5" t="s">
         <v>100</v>
       </c>
@@ -39875,7 +39876,7 @@
       <c r="BA61" s="106"/>
       <c r="BB61" s="105"/>
     </row>
-    <row r="62" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A62" s="129" t="s">
         <v>85</v>
       </c>
@@ -39949,7 +39950,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
         <v>86</v>
       </c>
@@ -40043,7 +40044,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
         <v>87</v>
       </c>
@@ -40354,7 +40355,7 @@
         <v>226.5</v>
       </c>
     </row>
-    <row r="66" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A66" s="5"/>
       <c r="B66" s="24"/>
       <c r="C66" s="24"/>
@@ -40603,7 +40604,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E43983A-2D59-5E42-8B10-50D25DDE0DB4}">
   <dimension ref="A1:BB67"/>
   <sheetViews>
     <sheetView zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="120" workbookViewId="0">
@@ -41365,7 +41366,7 @@
         <v>72.5</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A9" s="28" t="s">
         <v>58</v>
       </c>
@@ -43781,7 +43782,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
         <v>93</v>
       </c>
@@ -43888,7 +43889,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="32" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
         <v>83</v>
       </c>
@@ -45062,7 +45063,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="42" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A42" s="5" t="s">
         <v>23</v>
       </c>
@@ -45352,7 +45353,7 @@
       <c r="BA44" s="21"/>
       <c r="BB44" s="6"/>
     </row>
-    <row r="45" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A45" s="5" t="s">
         <v>25</v>
       </c>
@@ -46112,7 +46113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A51" s="5" t="s">
         <v>82</v>
       </c>
@@ -47053,7 +47054,7 @@
       <c r="BA58" s="16"/>
       <c r="BB58" s="8"/>
     </row>
-    <row r="59" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A59" s="5" t="s">
         <v>92</v>
       </c>
@@ -47149,7 +47150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A60" s="5" t="s">
         <v>99</v>
       </c>
@@ -47220,7 +47221,7 @@
       <c r="BA60" s="106"/>
       <c r="BB60" s="105"/>
     </row>
-    <row r="61" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A61" s="5" t="s">
         <v>100</v>
       </c>
@@ -47287,7 +47288,7 @@
       <c r="BA61" s="106"/>
       <c r="BB61" s="105"/>
     </row>
-    <row r="62" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A62" s="129" t="s">
         <v>85</v>
       </c>
@@ -47359,7 +47360,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
         <v>86</v>
       </c>
@@ -47453,7 +47454,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
         <v>87</v>
       </c>
@@ -47764,7 +47765,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A66" s="5"/>
       <c r="B66" s="24"/>
       <c r="C66" s="24"/>
@@ -48013,7 +48014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C1C5C9-025D-A34D-BC22-7DBC0940D30D}">
   <dimension ref="A1:BB67"/>
   <sheetViews>
     <sheetView zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="120" workbookViewId="0">
@@ -48757,7 +48758,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A9" s="28" t="s">
         <v>58</v>
       </c>
@@ -50595,7 +50596,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
         <v>93</v>
       </c>
@@ -50668,7 +50669,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
         <v>83</v>
       </c>
@@ -51646,7 +51647,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A42" s="5" t="s">
         <v>23</v>
       </c>
@@ -51858,7 +51859,7 @@
       <c r="BA44" s="21"/>
       <c r="BB44" s="6"/>
     </row>
-    <row r="45" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A45" s="5" t="s">
         <v>25</v>
       </c>
@@ -52550,7 +52551,7 @@
         <v>44.25</v>
       </c>
     </row>
-    <row r="51" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A51" s="5" t="s">
         <v>82</v>
       </c>
@@ -52955,7 +52956,7 @@
       <c r="AM54" s="19"/>
       <c r="BB54" s="6"/>
     </row>
-    <row r="55" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A55" s="5" t="s">
         <v>89</v>
       </c>
@@ -53017,7 +53018,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A56" s="129" t="s">
         <v>34</v>
       </c>
@@ -53357,7 +53358,7 @@
       <c r="BA58" s="16"/>
       <c r="BB58" s="8"/>
     </row>
-    <row r="59" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A59" s="5" t="s">
         <v>92</v>
       </c>
@@ -53415,7 +53416,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A60" s="5" t="s">
         <v>99</v>
       </c>
@@ -53466,7 +53467,7 @@
       <c r="BA60" s="106"/>
       <c r="BB60" s="105"/>
     </row>
-    <row r="61" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A61" s="5" t="s">
         <v>100</v>
       </c>
@@ -53517,7 +53518,7 @@
       <c r="BA61" s="106"/>
       <c r="BB61" s="105"/>
     </row>
-    <row r="62" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A62" s="129" t="s">
         <v>85</v>
       </c>
@@ -53569,7 +53570,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
         <v>86</v>
       </c>
@@ -53625,7 +53626,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
         <v>87</v>
       </c>
@@ -53898,7 +53899,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="66" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A66" s="5"/>
       <c r="B66" s="24"/>
       <c r="C66" s="24"/>
@@ -54147,7 +54148,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B6E99F-6F3A-9848-8213-283BACF02E4D}">
   <dimension ref="A1:BB67"/>
   <sheetViews>
     <sheetView zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="120" workbookViewId="0">
@@ -54906,7 +54907,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A9" s="28" t="s">
         <v>58</v>
       </c>
@@ -57320,7 +57321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
         <v>93</v>
       </c>
@@ -57427,7 +57428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
         <v>83</v>
       </c>
@@ -58601,7 +58602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A42" s="5" t="s">
         <v>23</v>
       </c>
@@ -58891,7 +58892,7 @@
       <c r="BA44" s="21"/>
       <c r="BB44" s="6"/>
     </row>
-    <row r="45" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A45" s="5" t="s">
         <v>25</v>
       </c>
@@ -59651,7 +59652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A51" s="5" t="s">
         <v>82</v>
       </c>
@@ -60124,7 +60125,7 @@
       <c r="AM54" s="19"/>
       <c r="BB54" s="6"/>
     </row>
-    <row r="55" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A55" s="5" t="s">
         <v>89</v>
       </c>
@@ -60220,7 +60221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A56" s="129" t="s">
         <v>34</v>
       </c>
@@ -60592,7 +60593,7 @@
       <c r="BA58" s="16"/>
       <c r="BB58" s="8"/>
     </row>
-    <row r="59" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A59" s="5" t="s">
         <v>92</v>
       </c>
@@ -60688,7 +60689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A60" s="5" t="s">
         <v>99</v>
       </c>
@@ -60759,7 +60760,7 @@
       <c r="BA60" s="106"/>
       <c r="BB60" s="105"/>
     </row>
-    <row r="61" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A61" s="5" t="s">
         <v>100</v>
       </c>
@@ -60826,7 +60827,7 @@
       <c r="BA61" s="106"/>
       <c r="BB61" s="105"/>
     </row>
-    <row r="62" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A62" s="129" t="s">
         <v>85</v>
       </c>
@@ -60898,7 +60899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
         <v>86</v>
       </c>
@@ -60992,7 +60993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
         <v>87</v>
       </c>
@@ -61303,7 +61304,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:54" ht="25" x14ac:dyDescent="0.4">
       <c r="A66" s="5"/>
       <c r="B66" s="24"/>
       <c r="C66" s="24"/>
@@ -61552,7 +61553,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C60D1D-BA10-6849-9804-12ED27A29108}">
   <dimension ref="A1:S67"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
@@ -61727,7 +61728,7 @@
       <c r="P7" s="47"/>
       <c r="Q7" s="48"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A8" s="50" t="s">
         <v>60</v>
       </c>
@@ -61934,7 +61935,7 @@
         <v>0.47578499201703034</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A11" s="50"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
@@ -61953,7 +61954,7 @@
       <c r="P11" s="52"/>
       <c r="Q11" s="53"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A12" s="50" t="s">
         <v>61</v>
       </c>
@@ -62022,7 +62023,7 @@
         <v>0.6211160431198478</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A13" s="121" t="s">
         <v>97</v>
       </c>
@@ -62091,7 +62092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A14" s="50" t="s">
         <v>62</v>
       </c>
@@ -62160,7 +62161,7 @@
         <v>0.51405071967100757</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A15" s="50" t="s">
         <v>63</v>
       </c>
@@ -62229,7 +62230,7 @@
         <v>0.64689063616869191</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A16" s="50" t="s">
         <v>64</v>
       </c>
@@ -62298,7 +62299,7 @@
         <v>0.51531841652323584</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A17" s="50" t="s">
         <v>76</v>
       </c>
@@ -62367,7 +62368,7 @@
         <v>0.65958572724523734</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A18" s="50" t="s">
         <v>59</v>
       </c>
@@ -62436,7 +62437,7 @@
         <v>0.71963095848282932</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A19" s="50" t="s">
         <v>77</v>
       </c>
@@ -62505,7 +62506,7 @@
         <v>0.61486486486486491</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A20" s="50" t="s">
         <v>84</v>
       </c>
@@ -62574,7 +62575,7 @@
         <v>0.65866388308977031</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A21" s="50" t="s">
         <v>65</v>
       </c>
@@ -62643,7 +62644,7 @@
         <v>0.76170046801872071</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A22" s="50" t="s">
         <v>79</v>
       </c>
@@ -62800,7 +62801,7 @@
       <c r="P24" s="52"/>
       <c r="Q24" s="53"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A25" s="114" t="s">
         <v>91</v>
       </c>
@@ -62869,7 +62870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A26" s="50" t="s">
         <v>66</v>
       </c>
@@ -62938,7 +62939,7 @@
         <v>0.48869680851063829</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A27" s="50" t="s">
         <v>67</v>
       </c>
@@ -63007,7 +63008,7 @@
         <v>0.52452352392376389</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A28" s="50" t="s">
         <v>95</v>
       </c>
@@ -63076,7 +63077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A29" s="50" t="s">
         <v>90</v>
       </c>
@@ -63145,7 +63146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A30" s="60" t="s">
         <v>80</v>
       </c>
@@ -63214,7 +63215,7 @@
         <v>0.88626392170097879</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A31" s="50" t="s">
         <v>68</v>
       </c>
@@ -63283,7 +63284,7 @@
         <v>0.83555420956995763</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:17" ht="17" x14ac:dyDescent="0.3">
       <c r="A32" s="50" t="s">
         <v>83</v>
       </c>
@@ -63352,7 +63353,7 @@
         <v>0.62950926226844328</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A33" s="50" t="s">
         <v>69</v>
       </c>
@@ -63421,7 +63422,7 @@
         <v>0.70154258886653253</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A34" s="58" t="s">
         <v>70</v>
       </c>
@@ -63490,7 +63491,7 @@
         <v>0.59204871060171915</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A35" s="58" t="s">
         <v>81</v>
       </c>
@@ -63628,7 +63629,7 @@
         <v>0.70394050365491434</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A37" s="50"/>
       <c r="B37" s="51"/>
       <c r="C37" s="51"/>
@@ -63647,7 +63648,7 @@
       <c r="P37" s="52"/>
       <c r="Q37" s="53"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A38" s="58" t="s">
         <v>71</v>
       </c>
@@ -63785,7 +63786,7 @@
         <v>0.56775700934579443</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A40" s="50"/>
       <c r="B40" s="51"/>
       <c r="C40" s="51"/>
@@ -63804,7 +63805,7 @@
       <c r="P40" s="52"/>
       <c r="Q40" s="53"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A41" s="50" t="s">
         <v>72</v>
       </c>
@@ -63873,7 +63874,7 @@
         <v>0.42109566639411283</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A42" s="50" t="s">
         <v>73</v>
       </c>
@@ -63942,7 +63943,7 @@
         <v>0.68174474959612275</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A43" s="50" t="s">
         <v>74</v>
       </c>
@@ -64011,7 +64012,7 @@
         <v>0.78647949759881786</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A44" s="121" t="s">
         <v>98</v>
       </c>
@@ -64080,7 +64081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A45" s="50" t="s">
         <v>75</v>
       </c>
@@ -64218,7 +64219,7 @@
         <v>0.58916102136529447</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="12" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="50"/>
       <c r="B47" s="51"/>
       <c r="C47" s="51"/>
@@ -64327,7 +64328,7 @@
       <c r="Q49" s="71"/>
       <c r="S49" s="72"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A50" s="50" t="s">
         <v>31</v>
       </c>
@@ -64396,7 +64397,7 @@
         <v>4.9502231376587706E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A51" s="50" t="s">
         <v>82</v>
       </c>
@@ -64465,7 +64466,7 @@
         <v>0.20219378427787935</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A52" s="50" t="s">
         <v>32</v>
       </c>
@@ -64603,7 +64604,7 @@
         <v>9.7624971725853882E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A54" s="50"/>
       <c r="B54" s="51"/>
       <c r="C54" s="51"/>
@@ -64622,7 +64623,7 @@
       <c r="P54" s="52"/>
       <c r="Q54" s="53"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A55" s="50" t="s">
         <v>89</v>
       </c>
@@ -64691,7 +64692,7 @@
         <v>0.24394184168012925</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A56" s="50" t="s">
         <v>34</v>
       </c>
@@ -64829,7 +64830,7 @@
         <v>0.37622756518794448</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A58" s="50"/>
       <c r="B58" s="51"/>
       <c r="J58" s="71"/>
@@ -64840,7 +64841,7 @@
       <c r="P58" s="101"/>
       <c r="Q58" s="71"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A59" s="50" t="s">
         <v>92</v>
       </c>
@@ -64909,7 +64910,7 @@
         <v>0.64433701657458564</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A60" s="121" t="s">
         <v>99</v>
       </c>
@@ -64978,7 +64979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A61" s="121" t="s">
         <v>100</v>
       </c>
@@ -65047,7 +65048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A62" s="50" t="s">
         <v>85</v>
       </c>
@@ -65116,7 +65117,7 @@
         <v>0.69117647058823528</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:19" ht="17" x14ac:dyDescent="0.3">
       <c r="A63" s="50" t="s">
         <v>86</v>
       </c>
@@ -65185,7 +65186,7 @@
         <v>0.6778221778221778</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="12" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="50" t="s">
         <v>87</v>
       </c>
@@ -65323,7 +65324,7 @@
         <v>0.75430413026884913</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="12" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="50"/>
     </row>
     <row r="67" spans="1:17" ht="13" thickBot="1" x14ac:dyDescent="0.2">

</xml_diff>